<commit_message>
The reporting form has been updated.
</commit_message>
<xml_diff>
--- a/Parameters/ProjectsAddInfo.xlsx
+++ b/Parameters/ProjectsAddInfo.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE44787B-E6BE-481B-A797-B970E5A39CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D47BA39-C1CA-4F30-956E-C886D4C81FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,16 +154,16 @@
     <t>Подр_Дек</t>
   </si>
   <si>
-    <t>С0588 - АСУ Погрузка</t>
-  </si>
-  <si>
-    <t>С0589 - ИС Информационная панель</t>
-  </si>
-  <si>
-    <t>Т0616 - 1-я линия: АСУ Погрузка</t>
-  </si>
-  <si>
-    <t>Т0617 - 1-я линия: ИС Информационная панель</t>
+    <t>Проект №2</t>
+  </si>
+  <si>
+    <t>Проект №3</t>
+  </si>
+  <si>
+    <t>Проект №4</t>
+  </si>
+  <si>
+    <t>Проект №1</t>
   </si>
 </sst>
 </file>
@@ -845,7 +845,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +933,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="17"/>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="20"/>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>

</xml_diff>

<commit_message>
Updates structure of data files.
</commit_message>
<xml_diff>
--- a/Parameters/ProjectsAddInfo.xlsx
+++ b/Parameters/ProjectsAddInfo.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D47BA39-C1CA-4F30-956E-C886D4C81FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC92DA67-6174-4E6A-ADF5-EBA564518E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Проект №5</t>
   </si>
@@ -152,6 +152,102 @@
   </si>
   <si>
     <t>Подр_Дек</t>
+  </si>
+  <si>
+    <t>Группа</t>
+  </si>
+  <si>
+    <t>Проект №21</t>
+  </si>
+  <si>
+    <t>Проект №22</t>
+  </si>
+  <si>
+    <t>Проект №23</t>
+  </si>
+  <si>
+    <t>Проект №24</t>
+  </si>
+  <si>
+    <t>Проект №25</t>
+  </si>
+  <si>
+    <t>Проект №26</t>
+  </si>
+  <si>
+    <t>Проект №27</t>
+  </si>
+  <si>
+    <t>Проект №28</t>
+  </si>
+  <si>
+    <t>Проект №29</t>
+  </si>
+  <si>
+    <t>Проект №30</t>
+  </si>
+  <si>
+    <t>Проект №31</t>
+  </si>
+  <si>
+    <t>Проект №32</t>
+  </si>
+  <si>
+    <t>Проект №33</t>
+  </si>
+  <si>
+    <t>Проект №34</t>
+  </si>
+  <si>
+    <t>Проект №35</t>
+  </si>
+  <si>
+    <t>Проект №36</t>
+  </si>
+  <si>
+    <t>Проект №37</t>
+  </si>
+  <si>
+    <t>Проект №38</t>
+  </si>
+  <si>
+    <t>Проект №39</t>
+  </si>
+  <si>
+    <t>Проект №40</t>
+  </si>
+  <si>
+    <t>Проект №41</t>
+  </si>
+  <si>
+    <t>Проект №42</t>
+  </si>
+  <si>
+    <t>Проект №43</t>
+  </si>
+  <si>
+    <t>Проект №44</t>
+  </si>
+  <si>
+    <t>Проект №45</t>
+  </si>
+  <si>
+    <t>Проект №46</t>
+  </si>
+  <si>
+    <t>Проект №47</t>
+  </si>
+  <si>
+    <t>Проект №48</t>
+  </si>
+  <si>
+    <t>Проект №49</t>
+  </si>
+  <si>
+    <t>Проект №50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
   <si>
     <t>Проект №2</t>
@@ -227,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -459,6 +555,50 @@
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="hair">
         <color auto="1"/>
       </top>
@@ -474,7 +614,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,6 +696,19 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -841,9 +994,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -851,389 +1004,218 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17">
-        <v>555000</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="17">
-        <v>555000</v>
-      </c>
+      <c r="G2" s="17"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="17">
-        <v>555000</v>
-      </c>
+      <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="18">
-        <v>555000</v>
-      </c>
-      <c r="N2" s="7">
-        <v>100</v>
-      </c>
-      <c r="O2" s="8">
-        <f>N2+100</f>
-        <v>200</v>
-      </c>
-      <c r="P2" s="8">
-        <f>O2+100</f>
-        <v>300</v>
-      </c>
-      <c r="Q2" s="8">
-        <f t="shared" ref="Q2:Y2" si="0">P2+100</f>
-        <v>400</v>
-      </c>
-      <c r="R2" s="8">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="S2" s="8">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="T2" s="8">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="U2" s="8">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="V2" s="8">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="W2" s="8">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="X2" s="8">
-        <f t="shared" si="0"/>
-        <v>1100</v>
-      </c>
-      <c r="Y2" s="9">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M2" s="17"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20">
-        <v>55500</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
-      <c r="G3" s="20">
-        <f>D3</f>
-        <v>55500</v>
-      </c>
+      <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
-      <c r="J3" s="20">
-        <f t="shared" ref="J3:J5" si="1">G3</f>
-        <v>55500</v>
-      </c>
+      <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
-      <c r="M3" s="21">
-        <f t="shared" ref="M3:M5" si="2">J3</f>
-        <v>55500</v>
-      </c>
-      <c r="N3" s="10">
-        <v>10</v>
-      </c>
-      <c r="O3" s="11">
-        <f t="shared" ref="O3:Y3" si="3">N3+100</f>
-        <v>110</v>
-      </c>
-      <c r="P3" s="11">
-        <f t="shared" si="3"/>
-        <v>210</v>
-      </c>
-      <c r="Q3" s="11">
-        <f t="shared" si="3"/>
-        <v>310</v>
-      </c>
-      <c r="R3" s="11">
-        <f t="shared" si="3"/>
-        <v>410</v>
-      </c>
-      <c r="S3" s="11">
-        <f t="shared" si="3"/>
-        <v>510</v>
-      </c>
-      <c r="T3" s="11">
-        <f t="shared" si="3"/>
-        <v>610</v>
-      </c>
-      <c r="U3" s="11">
-        <f t="shared" si="3"/>
-        <v>710</v>
-      </c>
-      <c r="V3" s="11">
-        <f t="shared" si="3"/>
-        <v>810</v>
-      </c>
-      <c r="W3" s="11">
-        <f t="shared" si="3"/>
-        <v>910</v>
-      </c>
-      <c r="X3" s="11">
-        <f t="shared" si="3"/>
-        <v>1010</v>
-      </c>
-      <c r="Y3" s="12">
-        <f t="shared" si="3"/>
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="12"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20">
-        <v>5550</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
-      <c r="G4" s="20">
-        <f t="shared" ref="G4:G5" si="4">D4</f>
-        <v>5550</v>
-      </c>
+      <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="20">
-        <f t="shared" si="1"/>
-        <v>5550</v>
-      </c>
+      <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
-      <c r="M4" s="21">
-        <f t="shared" si="2"/>
-        <v>5550</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="11">
-        <f t="shared" ref="O4:Y4" si="5">N4+100</f>
-        <v>101</v>
-      </c>
-      <c r="P4" s="11">
-        <f t="shared" si="5"/>
-        <v>201</v>
-      </c>
-      <c r="Q4" s="11">
-        <f t="shared" si="5"/>
-        <v>301</v>
-      </c>
-      <c r="R4" s="11">
-        <f t="shared" si="5"/>
-        <v>401</v>
-      </c>
-      <c r="S4" s="11">
-        <f t="shared" si="5"/>
-        <v>501</v>
-      </c>
-      <c r="T4" s="11">
-        <f t="shared" si="5"/>
-        <v>601</v>
-      </c>
-      <c r="U4" s="11">
-        <f t="shared" si="5"/>
-        <v>701</v>
-      </c>
-      <c r="V4" s="11">
-        <f t="shared" si="5"/>
-        <v>801</v>
-      </c>
-      <c r="W4" s="11">
-        <f t="shared" si="5"/>
-        <v>901</v>
-      </c>
-      <c r="X4" s="11">
-        <f t="shared" si="5"/>
-        <v>1001</v>
-      </c>
-      <c r="Y4" s="12">
-        <f t="shared" si="5"/>
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20">
-        <v>555</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="20">
-        <f t="shared" si="4"/>
-        <v>555</v>
-      </c>
+      <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="20">
-        <f t="shared" si="1"/>
-        <v>555</v>
-      </c>
+      <c r="J5" s="20"/>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
-      <c r="M5" s="21">
-        <f t="shared" si="2"/>
-        <v>555</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="11">
-        <f t="shared" ref="O5:Y5" si="6">N5+100</f>
-        <v>100.5</v>
-      </c>
-      <c r="P5" s="11">
-        <f t="shared" si="6"/>
-        <v>200.5</v>
-      </c>
-      <c r="Q5" s="11">
-        <f t="shared" si="6"/>
-        <v>300.5</v>
-      </c>
-      <c r="R5" s="11">
-        <f t="shared" si="6"/>
-        <v>400.5</v>
-      </c>
-      <c r="S5" s="11">
-        <f t="shared" si="6"/>
-        <v>500.5</v>
-      </c>
-      <c r="T5" s="11">
-        <f t="shared" si="6"/>
-        <v>600.5</v>
-      </c>
-      <c r="U5" s="11">
-        <f t="shared" si="6"/>
-        <v>700.5</v>
-      </c>
-      <c r="V5" s="11">
-        <f t="shared" si="6"/>
-        <v>800.5</v>
-      </c>
-      <c r="W5" s="11">
-        <f t="shared" si="6"/>
-        <v>900.5</v>
-      </c>
-      <c r="X5" s="11">
-        <f t="shared" si="6"/>
-        <v>1000.5</v>
-      </c>
-      <c r="Y5" s="12">
-        <f t="shared" si="6"/>
-        <v>1100.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -1243,9 +1225,9 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="11"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="10"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -1255,14 +1237,15 @@
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
-      <c r="Y6" s="12"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="12"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -1272,9 +1255,9 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="10"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -1284,14 +1267,15 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="11"/>
-      <c r="Y7" s="12"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="12"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -1301,9 +1285,9 @@
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
@@ -1313,14 +1297,15 @@
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="11"/>
-      <c r="Y8" s="12"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="12"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
@@ -1330,9 +1315,9 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
@@ -1342,14 +1327,15 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
-      <c r="Y9" s="12"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="12"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -1359,9 +1345,9 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="11"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
@@ -1371,14 +1357,15 @@
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
-      <c r="Y10" s="12"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="12"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -1388,9 +1375,9 @@
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="11"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
@@ -1400,14 +1387,15 @@
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
-      <c r="Y11" s="12"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="12"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -1417,9 +1405,9 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="11"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="10"/>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
@@ -1429,14 +1417,15 @@
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
-      <c r="Y12" s="12"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="12"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
@@ -1446,9 +1435,9 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="11"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="10"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
@@ -1458,14 +1447,15 @@
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
-      <c r="Y13" s="12"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="12"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -1475,9 +1465,9 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="11"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="10"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
@@ -1487,14 +1477,15 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
-      <c r="Y14" s="12"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="12"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -1504,9 +1495,9 @@
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="11"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
@@ -1516,14 +1507,15 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
-      <c r="Y15" s="12"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="12"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -1533,9 +1525,9 @@
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="11"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="10"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -1545,14 +1537,15 @@
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
-      <c r="Y16" s="12"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="12"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -1562,9 +1555,9 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="11"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="10"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -1574,14 +1567,15 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
-      <c r="Y17" s="12"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="12"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
@@ -1591,9 +1585,9 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="11"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="10"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
@@ -1603,14 +1597,15 @@
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
-      <c r="Y18" s="12"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="12"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -1620,9 +1615,9 @@
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="11"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="10"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -1632,14 +1627,15 @@
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
-      <c r="Y19" s="12"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="12"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1649,9 +1645,9 @@
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="11"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="10"/>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -1661,45 +1657,947 @@
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
-      <c r="Y20" s="12"/>
-    </row>
-    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="12"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="15"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="12"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="12"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="12"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="12"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="12"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="31"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="12"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="12"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="31"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="12"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="12"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="12"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="12"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="12"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="12"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="31"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="12"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="12"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="12"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="31"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="12"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="12"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="12"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="31"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="12"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="12"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="31"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="12"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="12"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="31"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="12"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="31"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="12"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="31"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="12"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="31"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="12"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="31"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
+      <c r="Z48" s="12"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
+      <c r="Z49" s="12"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="31"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
+      <c r="Z50" s="12"/>
+    </row>
+    <row r="51" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="32"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:Y21" xr:uid="{12ECEA5A-5684-46AB-AD36-142C9F78A0DF}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:Z51" xr:uid="{12ECEA5A-5684-46AB-AD36-142C9F78A0DF}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>